<commit_message>
Value Document // Purcahse Corrections // Max Ammo
Filling out the document before my ass goes to bed Also some Ammo corrections. Max Ammo wasn't set for Nitro. Also some corrections for Buy Values
</commit_message>
<xml_diff>
--- a/Map 1 - Gun Damage, Explosive, and Trap Values Values.xlsx
+++ b/Map 1 - Gun Damage, Explosive, and Trap Values Values.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
   <si>
     <t>Guns</t>
   </si>
@@ -84,13 +84,253 @@
   </si>
   <si>
     <t>Reload Speed</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Cost, Upgraded Cost</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Bullets</t>
+  </si>
+  <si>
+    <t>Bullet</t>
+  </si>
+  <si>
+    <t>Explosion</t>
+  </si>
+  <si>
+    <t>200 Ammo, 500 Ammo Upgraded</t>
+  </si>
+  <si>
+    <t>20, 45 Upgraded</t>
+  </si>
+  <si>
+    <t>45, 80 Upgraded</t>
+  </si>
+  <si>
+    <t>Proximity Trigger of within 50</t>
+  </si>
+  <si>
+    <t>1k,2k, 3k</t>
+  </si>
+  <si>
+    <t>150, 100, 50, 25</t>
+  </si>
+  <si>
+    <t>Remote Trigger -  35, 70, 105, 140</t>
+  </si>
+  <si>
+    <t>250, 400</t>
+  </si>
+  <si>
+    <t>250, 450</t>
+  </si>
+  <si>
+    <t>200, 250</t>
+  </si>
+  <si>
+    <t>Infinite</t>
+  </si>
+  <si>
+    <t>Mouse Click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 frames </t>
+  </si>
+  <si>
+    <t>30 frames</t>
+  </si>
+  <si>
+    <t>Free, 1250 (Auto Pistol Upgraded)</t>
+  </si>
+  <si>
+    <t>Shotgun</t>
+  </si>
+  <si>
+    <t>Mosin Nagant (Sniper)</t>
+  </si>
+  <si>
+    <t>MP9</t>
+  </si>
+  <si>
+    <t>Bolt-Action</t>
+  </si>
+  <si>
+    <t>Semi -Auto</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Pump Action</t>
+  </si>
+  <si>
+    <t>M60</t>
+  </si>
+  <si>
+    <t>Desert Eagle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouse Click </t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>FNFAL</t>
+  </si>
+  <si>
+    <t>AK12</t>
+  </si>
+  <si>
+    <t>Scorcher</t>
+  </si>
+  <si>
+    <t>XL79</t>
+  </si>
+  <si>
+    <t>MG42</t>
+  </si>
+  <si>
+    <t>AT4</t>
+  </si>
+  <si>
+    <t>AA12</t>
+  </si>
+  <si>
+    <t>Nitro</t>
+  </si>
+  <si>
+    <t>50 BMG</t>
+  </si>
+  <si>
+    <t>Minigun</t>
+  </si>
+  <si>
+    <t>HOD</t>
+  </si>
+  <si>
+    <t>DROPOGM</t>
+  </si>
+  <si>
+    <t>3-Round Burst</t>
+  </si>
+  <si>
+    <t>One Shot</t>
+  </si>
+  <si>
+    <t>Pistol (Auto when upgraded)</t>
+  </si>
+  <si>
+    <t>60 frames</t>
+  </si>
+  <si>
+    <t>90 Frames</t>
+  </si>
+  <si>
+    <t>8 Frames</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>45 frames</t>
+  </si>
+  <si>
+    <t>8 frames</t>
+  </si>
+  <si>
+    <t>40 Frames</t>
+  </si>
+  <si>
+    <t>10 frames</t>
+  </si>
+  <si>
+    <t>6 Frames</t>
+  </si>
+  <si>
+    <t>180 Frames</t>
+  </si>
+  <si>
+    <t>4 frames per shot 8 frames for all 3</t>
+  </si>
+  <si>
+    <t>30 Frames</t>
+  </si>
+  <si>
+    <t>45 Frames</t>
+  </si>
+  <si>
+    <t>120 Frames</t>
+  </si>
+  <si>
+    <t>10 Frames</t>
+  </si>
+  <si>
+    <t>2 Frames</t>
+  </si>
+  <si>
+    <t>210 Frames</t>
+  </si>
+  <si>
+    <t>60 Frames</t>
+  </si>
+  <si>
+    <t>300 Frames</t>
+  </si>
+  <si>
+    <t>1500 Health</t>
+  </si>
+  <si>
+    <t>1875 Health</t>
+  </si>
+  <si>
+    <t>500 Health</t>
+  </si>
+  <si>
+    <t>625 Health</t>
+  </si>
+  <si>
+    <t>30 Per Pellet</t>
+  </si>
+  <si>
+    <t>45 Per Pellet</t>
+  </si>
+  <si>
+    <t>40 Per Pellet</t>
+  </si>
+  <si>
+    <t>55 Per Pellet</t>
+  </si>
+  <si>
+    <t>150,115,80,75</t>
+  </si>
+  <si>
+    <t>1 Frame/ 35,70,105,140  Up 50,85,120,135</t>
+  </si>
+  <si>
+    <t>1 Frame / 35,70,105,140 Up 50,85,120,155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.5 Frames </t>
+  </si>
+  <si>
+    <t>9 Frames / 35,70,105,140 Up 50,85,120,155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90 Frames </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +345,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -114,7 +361,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,13 +369,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,92 +669,777 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>12.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>450</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>37.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>43.75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>108</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>62.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>450</v>
+      </c>
+      <c r="D9">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <v>43.75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>400</v>
+      </c>
+      <c r="D10">
+        <v>35</v>
+      </c>
+      <c r="E10">
+        <v>43.75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>450</v>
+      </c>
+      <c r="D11">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>43.75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12">
+        <v>250</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>15.75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="2">
+        <v>200165130100</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14">
+        <v>200</v>
+      </c>
+      <c r="C14">
+        <v>1000</v>
+      </c>
+      <c r="D14">
+        <v>45</v>
+      </c>
+      <c r="E14">
+        <v>78.75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2">
+        <v>225190155120</v>
+      </c>
+      <c r="E15" s="2">
+        <v>275240205165</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2">
+        <v>40</v>
+      </c>
+      <c r="E17" s="2">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>115</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19">
+        <v>500</v>
+      </c>
+      <c r="C19">
+        <v>2000</v>
+      </c>
+      <c r="D19" s="2">
+        <v>35</v>
+      </c>
+      <c r="E19" s="2">
+        <v>43.75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>900</v>
+      </c>
+      <c r="D20">
+        <v>300</v>
+      </c>
+      <c r="E20">
+        <v>375</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="2">
+        <v>300250200175</v>
+      </c>
+      <c r="E21" s="2">
+        <v>350300250215</v>
+      </c>
+      <c r="F21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H26" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="I26" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+      <c r="E28">
+        <v>150</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Documents / Value Changes
Added document for ideas for the next maps /
</commit_message>
<xml_diff>
--- a/Map 1 - Gun Damage, Explosive, and Trap Values Values.xlsx
+++ b/Map 1 - Gun Damage, Explosive, and Trap Values Values.xlsx
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +754,7 @@
         <v>30</v>
       </c>
       <c r="C3">
-        <v>450</v>
+        <v>360</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -783,7 +783,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
         <v>90</v>
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
         <v>88</v>
@@ -841,7 +841,7 @@
         <v>30</v>
       </c>
       <c r="C6">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -1131,7 +1131,7 @@
         <v>20</v>
       </c>
       <c r="C16">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D16" t="s">
         <v>92</v>
@@ -1160,7 +1160,7 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D17" s="2">
         <v>40</v>
@@ -1276,7 +1276,7 @@
         <v>10</v>
       </c>
       <c r="C21">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="D21" s="2">
         <v>300250200175</v>

</xml_diff>